<commit_message>
merged yesterday's periya's and parvathy's changes with Lekshmi's code
</commit_message>
<xml_diff>
--- a/New Framework (Non-IWAF)/Android/UOM_Android_JSN/DataPool.xlsx
+++ b/New Framework (Non-IWAF)/Android/UOM_Android_JSN/DataPool.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MrDon/Documents/Android/UOM_Android_JSN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parvathy_p/Documents/workspace/uom-automation/New Framework (Non-IWAF)/Android/UOM_Android_JSN/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -883,7 +880,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
OffshoreQA script rework updates
</commit_message>
<xml_diff>
--- a/New Framework (Non-IWAF)/Android/UOM_Android_JSN/DataPool.xlsx
+++ b/New Framework (Non-IWAF)/Android/UOM_Android_JSN/DataPool.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="153">
   <si>
     <t>welcome1</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>012310</t>
+  </si>
+  <si>
+    <t>squomsa39</t>
   </si>
 </sst>
 </file>
@@ -877,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1164,6 +1167,74 @@
       <c r="C25" s="5" t="s">
         <v>131</v>
       </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5">
+        <v>719179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>